<commit_message>
Ajuste no service, business e MVC para BUG #22 da planilha de Atividades: Fazer tratamento para que quando eu convide algum usuário, ao entrar no perfil dele, invés de aparecer pra adicionar de novo, apareça algo do tipo "Aguardando resposta de amizade."
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.dinarte\Documents\fusioness\Trunk\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="11340" windowHeight="6285"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="11340" windowHeight="6285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5" sheetId="2" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>Responsável</t>
   </si>
@@ -378,8 +383,6 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -401,135 +404,18 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -550,28 +436,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -652,14 +517,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -697,9 +565,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -734,7 +602,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -769,7 +637,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -945,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -962,10 +830,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="4"/>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -990,13 +858,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1005,13 +873,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1020,13 +888,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1035,13 +903,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1050,13 +918,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1065,13 +933,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1080,10 +948,10 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:B11">
-    <cfRule type="cellIs" dxfId="18" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1093,10 +961,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1112,10 +981,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="3"/>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1135,15 +1004,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="13" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="8"/>
@@ -1155,111 +1024,111 @@
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>4</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>61</v>
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>6</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>7</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="13" t="s">
         <v>41</v>
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>8</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="14" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>9</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="13" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="8"/>
@@ -1271,10 +1140,10 @@
       <c r="B15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="8"/>
@@ -1286,10 +1155,10 @@
       <c r="B16" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="9"/>
@@ -1301,10 +1170,10 @@
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="8"/>
@@ -1316,10 +1185,10 @@
       <c r="B18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="9"/>
@@ -1331,66 +1200,66 @@
       <c r="B19" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>15</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="14" t="s">
         <v>45</v>
       </c>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>16</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="13" t="s">
         <v>61</v>
       </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="14" t="s">
         <v>62</v>
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>18</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="13" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="8"/>
@@ -1402,36 +1271,36 @@
       <c r="B24" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>20</v>
       </c>
       <c r="B25" s="9"/>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="14" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>21</v>
       </c>
       <c r="B26" s="9"/>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="13" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="8"/>
@@ -1440,24 +1309,26 @@
       <c r="A27" s="9">
         <v>22</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="14" t="s">
+      <c r="B27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>23</v>
       </c>
       <c r="B28" s="9"/>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E28" s="8"/>
@@ -1467,10 +1338,10 @@
         <v>24</v>
       </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="9"/>
@@ -1480,23 +1351,23 @@
         <v>25</v>
       </c>
       <c r="B30" s="9"/>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>26</v>
       </c>
       <c r="B31" s="9"/>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="14" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="9"/>
@@ -1506,10 +1377,10 @@
         <v>27</v>
       </c>
       <c r="B32" s="9"/>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E32" s="8"/>
@@ -1519,36 +1390,36 @@
         <v>28</v>
       </c>
       <c r="B33" s="9"/>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>29</v>
       </c>
       <c r="B34" s="9"/>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E35" s="8"/>
@@ -1558,62 +1429,62 @@
         <v>31</v>
       </c>
       <c r="B36" s="9"/>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>32</v>
       </c>
       <c r="B37" s="9"/>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="13" t="s">
         <v>43</v>
       </c>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>33</v>
       </c>
       <c r="B38" s="9"/>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="14" t="s">
         <v>43</v>
       </c>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>34</v>
       </c>
       <c r="B39" s="9"/>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="13" t="s">
         <v>45</v>
       </c>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>35</v>
       </c>
       <c r="B40" s="9"/>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="14" t="s">
         <v>45</v>
       </c>
       <c r="E40" s="9"/>
@@ -1623,25 +1494,31 @@
         <v>36</v>
       </c>
       <c r="B41" s="9"/>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E41" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:E41"/>
+  <autoFilter ref="A5:E41">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Douglas Dinarte"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B6:B41">
-    <cfRule type="cellIs" dxfId="22" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Alterações para correção de bugs encontrados. Atualizada a planilha de Atividades da Sprint #5 com a descrição dos bugs.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.dinarte\Documents\fusioness\Trunk\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\fusioness\Trunk\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,14 +16,14 @@
     <sheet name="To-do list" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$E$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$F$41</definedName>
   </definedNames>
   <calcPr calcId="101716" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
   <si>
     <t>Responsável</t>
   </si>
@@ -259,6 +259,24 @@
   </si>
   <si>
     <t>Tarcísio</t>
+  </si>
+  <si>
+    <t>Criticidade</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Falta apenas adicionar pra ver os contatos deste usuário.</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Marcus Vinícius</t>
   </si>
 </sst>
 </file>
@@ -268,7 +286,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -299,6 +317,12 @@
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -357,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -404,8 +428,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,9 +553,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -565,7 +593,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -637,7 +665,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -814,7 +842,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -830,10 +858,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="20"/>
       <c r="D1" s="4"/>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -962,10 +990,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -973,21 +1001,23 @@
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="60.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="19.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="20"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -998,13 +1028,16 @@
         <v>35</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1013,11 +1046,14 @@
         <v>46</v>
       </c>
       <c r="D6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1027,12 +1063,13 @@
       <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1042,12 +1079,13 @@
       <c r="C8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1057,12 +1095,13 @@
       <c r="C9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1072,25 +1111,33 @@
       <c r="C10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>6</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C11" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -1099,11 +1146,14 @@
         <v>49</v>
       </c>
       <c r="D12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -1113,12 +1163,13 @@
       <c r="C13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>9</v>
       </c>
@@ -1128,12 +1179,13 @@
       <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -1143,12 +1195,13 @@
       <c r="C15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="13"/>
+      <c r="E15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" ht="76.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>11</v>
       </c>
@@ -1158,12 +1211,13 @@
       <c r="C16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13"/>
+      <c r="E16" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>12</v>
       </c>
@@ -1173,12 +1227,13 @@
       <c r="C17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="13"/>
+      <c r="E17" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>13</v>
       </c>
@@ -1188,12 +1243,13 @@
       <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13"/>
+      <c r="E18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" ht="114.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>14</v>
       </c>
@@ -1203,12 +1259,13 @@
       <c r="C19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="13"/>
+      <c r="E19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -1218,25 +1275,31 @@
       <c r="C20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>16</v>
       </c>
-      <c r="B21" s="9"/>
+      <c r="B21" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C21" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>17</v>
       </c>
@@ -1244,12 +1307,15 @@
       <c r="C22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>18</v>
       </c>
@@ -1259,12 +1325,13 @@
       <c r="C23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>19</v>
       </c>
@@ -1274,25 +1341,31 @@
       <c r="C24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="13"/>
+      <c r="E24" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>20</v>
       </c>
-      <c r="B25" s="9"/>
+      <c r="B25" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C25" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>21</v>
       </c>
@@ -1301,11 +1374,14 @@
         <v>21</v>
       </c>
       <c r="D26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>22</v>
       </c>
@@ -1315,12 +1391,13 @@
       <c r="C27" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13"/>
+      <c r="E27" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>23</v>
       </c>
@@ -1329,11 +1406,14 @@
         <v>23</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>24</v>
       </c>
@@ -1341,12 +1421,15 @@
       <c r="C29" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>25</v>
       </c>
@@ -1355,11 +1438,14 @@
         <v>24</v>
       </c>
       <c r="D30" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>26</v>
       </c>
@@ -1367,38 +1453,47 @@
       <c r="C31" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>27</v>
       </c>
-      <c r="B32" s="9"/>
+      <c r="B32" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C32" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="13"/>
+      <c r="E32" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>28</v>
       </c>
-      <c r="B33" s="9"/>
+      <c r="B33" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C33" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="13"/>
+      <c r="E33" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>29</v>
       </c>
@@ -1406,12 +1501,15 @@
       <c r="C34" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>30</v>
       </c>
@@ -1420,24 +1518,30 @@
         <v>29</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>31</v>
       </c>
-      <c r="B36" s="9"/>
+      <c r="B36" s="21"/>
       <c r="C36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>32</v>
       </c>
@@ -1446,11 +1550,14 @@
         <v>47</v>
       </c>
       <c r="D37" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>33</v>
       </c>
@@ -1458,12 +1565,15 @@
       <c r="C38" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" spans="1:5" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>34</v>
       </c>
@@ -1472,11 +1582,14 @@
         <v>32</v>
       </c>
       <c r="D39" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>35</v>
       </c>
@@ -1484,30 +1597,34 @@
       <c r="C40" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>36</v>
       </c>
-      <c r="B41" s="9"/>
+      <c r="B41" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C41" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="11"/>
+      <c r="E41" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:E41">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Douglas Dinarte"/>
-      </filters>
+  <autoFilter ref="A5:F41">
+    <filterColumn colId="1">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Atualizacao da Planilha Atividades Sprint #5.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.dinarte\Documents\fusioness\Trunk\Doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="11340" windowHeight="6285" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5" sheetId="2" r:id="rId1"/>
@@ -19,11 +14,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$E$41</definedName>
   </definedNames>
   <calcPr calcId="101716" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
   <si>
     <t>Responsável</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>Tarcísio</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>Convidar amigo por email agora é async</t>
+  </si>
+  <si>
+    <t>Convidar amigo por email agora aceita mais de um email, separados por vírgula. Obs: com validação.</t>
   </si>
 </sst>
 </file>
@@ -268,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -301,6 +310,18 @@
       <color indexed="9"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -339,23 +360,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -407,11 +436,75 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="10">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -567,7 +660,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,7 +695,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -811,32 +904,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="41.25" customHeight="1">
       <c r="B1" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -853,7 +946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="39">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -868,7 +961,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="26">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -883,7 +976,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="26">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -898,7 +991,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="26">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -913,11 +1006,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="26">
       <c r="A10" s="6">
         <v>5</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="C10" s="11" t="s">
         <v>52</v>
       </c>
@@ -928,7 +1023,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="52">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -942,12 +1037,58 @@
       <c r="E11" s="12" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="12" spans="1:5" ht="26">
+      <c r="A12" s="6">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:B11">
+    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
     <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
@@ -956,38 +1097,44 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="41.25" customHeight="1">
       <c r="B1" s="18" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1004,7 +1151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="78" hidden="1">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1017,7 +1164,7 @@
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="65">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1032,7 +1179,7 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="38.25" hidden="1" customHeight="1">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1047,7 +1194,7 @@
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="39" hidden="1">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1062,7 +1209,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="39" hidden="1">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1077,7 +1224,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="26" hidden="1">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1090,7 +1237,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="65" hidden="1">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -1103,7 +1250,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="102" hidden="1" customHeight="1">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -1118,7 +1265,7 @@
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="52" hidden="1">
       <c r="A14" s="6">
         <v>9</v>
       </c>
@@ -1133,7 +1280,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="89.25" customHeight="1">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -1148,7 +1295,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="76.5" customHeight="1">
       <c r="A16" s="6">
         <v>11</v>
       </c>
@@ -1163,7 +1310,7 @@
       </c>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="102" customHeight="1">
       <c r="A17" s="9">
         <v>12</v>
       </c>
@@ -1178,7 +1325,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="65">
       <c r="A18" s="6">
         <v>13</v>
       </c>
@@ -1193,7 +1340,7 @@
       </c>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="114.75" customHeight="1">
       <c r="A19" s="9">
         <v>14</v>
       </c>
@@ -1208,7 +1355,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="63.75" hidden="1" customHeight="1">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -1223,7 +1370,7 @@
       </c>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="26" hidden="1">
       <c r="A21" s="9">
         <v>16</v>
       </c>
@@ -1236,7 +1383,7 @@
       </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" hidden="1">
       <c r="A22" s="6">
         <v>17</v>
       </c>
@@ -1249,7 +1396,7 @@
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" hidden="1">
       <c r="A23" s="9">
         <v>18</v>
       </c>
@@ -1264,7 +1411,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="6">
         <v>19</v>
       </c>
@@ -1279,7 +1426,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="26" hidden="1">
       <c r="A25" s="9">
         <v>20</v>
       </c>
@@ -1292,7 +1439,7 @@
       </c>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="26" hidden="1">
       <c r="A26" s="6">
         <v>21</v>
       </c>
@@ -1305,7 +1452,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="39">
       <c r="A27" s="9">
         <v>22</v>
       </c>
@@ -1320,7 +1467,7 @@
       </c>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="26" hidden="1">
       <c r="A28" s="6">
         <v>23</v>
       </c>
@@ -1333,7 +1480,7 @@
       </c>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="26">
       <c r="A29" s="9">
         <v>24</v>
       </c>
@@ -1346,7 +1493,7 @@
       </c>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" s="6">
         <v>25</v>
       </c>
@@ -1359,7 +1506,7 @@
       </c>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="65" hidden="1">
       <c r="A31" s="9">
         <v>26</v>
       </c>
@@ -1372,7 +1519,7 @@
       </c>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="39">
       <c r="A32" s="6">
         <v>27</v>
       </c>
@@ -1385,7 +1532,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="26">
       <c r="A33" s="9">
         <v>28</v>
       </c>
@@ -1398,7 +1545,7 @@
       </c>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:5" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="63.75" hidden="1" customHeight="1">
       <c r="A34" s="6">
         <v>29</v>
       </c>
@@ -1411,7 +1558,7 @@
       </c>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="26" hidden="1">
       <c r="A35" s="9">
         <v>30</v>
       </c>
@@ -1424,7 +1571,7 @@
       </c>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="26">
       <c r="A36" s="6">
         <v>31</v>
       </c>
@@ -1437,7 +1584,7 @@
       </c>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="26" hidden="1">
       <c r="A37" s="9">
         <v>32</v>
       </c>
@@ -1450,7 +1597,7 @@
       </c>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" hidden="1">
       <c r="A38" s="6">
         <v>33</v>
       </c>
@@ -1463,7 +1610,7 @@
       </c>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="1:5" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="39" hidden="1">
       <c r="A39" s="9">
         <v>34</v>
       </c>
@@ -1476,7 +1623,7 @@
       </c>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="26" hidden="1">
       <c r="A40" s="6">
         <v>35</v>
       </c>
@@ -1489,7 +1636,7 @@
       </c>
       <c r="E40" s="9"/>
     </row>
-    <row r="41" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="26">
       <c r="A41" s="9">
         <v>36</v>
       </c>
@@ -1515,15 +1662,20 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B6:B41">
-    <cfRule type="cellIs" dxfId="1" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização dos bugs com desenvolvimento de correções. Atualização da planilha de acompanhamento das atividades.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="11340" windowHeight="6285"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="11340" windowHeight="6285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5" sheetId="2" r:id="rId1"/>
     <sheet name="To-do list" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$F$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$F$50</definedName>
   </definedNames>
   <calcPr calcId="101716" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="74">
   <si>
     <t>Responsável</t>
   </si>
@@ -164,9 +164,6 @@
     <t>No menu Buscar Contatos, a tela já abre listando todos os contatos da base, a tela deve abrir fazia e o usuario filtrar(ao consultar não deve aparecer ele mesmo e nem seu contatos)</t>
   </si>
   <si>
-    <t>Na tela de detalhe dos eventos, exibir uma lista com os usuários participantes daquele evento.</t>
-  </si>
-  <si>
     <t>Na tela de criar evento, ajustar o título para Criação de Eventos ao invés de Detalhe de Evento.</t>
   </si>
   <si>
@@ -277,6 +274,24 @@
   </si>
   <si>
     <t>Marcus Vinícius</t>
+  </si>
+  <si>
+    <t>Verificar a questão de paginação das páginas que contenham lista.</t>
+  </si>
+  <si>
+    <t>Na tela de detalhe dos eventos, exibir uma lista com os usuários participantes daquele evento. Nesta lista pode entrar também alguns detalhes e estatísticas.</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Fazer tratamento HTML para que o tamanho da imagem do evento seja padrão.</t>
+  </si>
+  <si>
+    <t>Verificar o erro que aconteceu ao alterar um evento.</t>
+  </si>
+  <si>
+    <t>No lugar de escolher a rota para o evento, colocar uma seleção onde se possa ver os mapas das rotas possíveis.</t>
   </si>
 </sst>
 </file>
@@ -381,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -432,6 +447,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -439,7 +457,133 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -841,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -858,10 +1002,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="21"/>
+      <c r="B1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="22"/>
       <c r="D1" s="4"/>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -872,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>0</v>
@@ -889,13 +1033,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -904,13 +1048,13 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -919,13 +1063,13 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
@@ -934,13 +1078,13 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -951,13 +1095,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -968,13 +1112,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -982,10 +1126,10 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:B11">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -995,11 +1139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1016,10 +1159,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="21"/>
+      <c r="B1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="22"/>
       <c r="D1" s="18"/>
       <c r="E1" s="3"/>
     </row>
@@ -1031,10 +1174,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>0</v>
@@ -1043,7 +1186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1051,17 +1194,17 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1073,11 +1216,11 @@
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1089,11 +1232,11 @@
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1105,11 +1248,11 @@
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1121,11 +1264,11 @@
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1133,19 +1276,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -1153,17 +1296,17 @@
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -1175,11 +1318,11 @@
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>9</v>
       </c>
@@ -1191,11 +1334,11 @@
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -1207,11 +1350,11 @@
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="76.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>11</v>
       </c>
@@ -1223,11 +1366,11 @@
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>12</v>
       </c>
@@ -1239,11 +1382,11 @@
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>13</v>
       </c>
@@ -1255,11 +1398,11 @@
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="114.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>14</v>
       </c>
@@ -1271,11 +1414,11 @@
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -1287,11 +1430,11 @@
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>16</v>
       </c>
@@ -1302,10 +1445,10 @@
         <v>17</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -1318,14 +1461,14 @@
         <v>18</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>18</v>
       </c>
@@ -1337,11 +1480,11 @@
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>19</v>
       </c>
@@ -1353,11 +1496,11 @@
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>20</v>
       </c>
@@ -1365,13 +1508,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F25" s="9"/>
     </row>
@@ -1379,19 +1522,21 @@
       <c r="A26" s="6">
         <v>21</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C26" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>22</v>
       </c>
@@ -1403,7 +1548,7 @@
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" s="9"/>
     </row>
@@ -1416,10 +1561,10 @@
         <v>23</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" s="8"/>
     </row>
@@ -1432,10 +1577,10 @@
         <v>25</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F29" s="9"/>
     </row>
@@ -1443,15 +1588,17 @@
       <c r="A30" s="6">
         <v>25</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C30" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="8"/>
     </row>
@@ -1461,17 +1608,17 @@
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>27</v>
       </c>
@@ -1483,11 +1630,11 @@
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>28</v>
       </c>
@@ -1499,11 +1646,11 @@
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>29</v>
       </c>
@@ -1514,14 +1661,14 @@
         <v>28</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>30</v>
       </c>
@@ -1532,10 +1679,10 @@
         <v>29</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="8"/>
     </row>
@@ -1543,15 +1690,17 @@
       <c r="A36" s="6">
         <v>31</v>
       </c>
-      <c r="B36" s="19"/>
+      <c r="B36" s="19" t="s">
+        <v>1</v>
+      </c>
       <c r="C36" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F36" s="9"/>
     </row>
@@ -1561,13 +1710,13 @@
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F37" s="8"/>
     </row>
@@ -1580,10 +1729,10 @@
         <v>31</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F38" s="9"/>
     </row>
@@ -1596,30 +1745,30 @@
         <v>32</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>35</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="12" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>36</v>
       </c>
@@ -1627,29 +1776,211 @@
         <v>1</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F41" s="8"/>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>36</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>36</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>36</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>36</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="9">
+        <v>36</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>36</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
+        <v>36</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>36</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>36</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A5:F41">
-    <filterColumn colId="1">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A5:F50"/>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B6:B41">
-    <cfRule type="cellIs" dxfId="1" priority="11" stopIfTrue="1" operator="notEqual">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="29" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="30" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="cellIs" dxfId="17" priority="17" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="cellIs" dxfId="15" priority="15" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Atualização do sprint backlog e status do bugfix
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="11340" windowHeight="6285" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="140" windowWidth="20940" windowHeight="16720"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5" sheetId="2" r:id="rId1"/>
@@ -14,11 +14,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$F$45</definedName>
   </definedNames>
   <calcPr calcId="101716" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="78">
   <si>
     <t>Responsável</t>
   </si>
@@ -287,6 +292,18 @@
   </si>
   <si>
     <t>No lugar de escolher a rota para o evento, colocar uma seleção onde se possa ver os mapas das rotas possíveis.</t>
+  </si>
+  <si>
+    <t>Remoção do hotlink das imagens de background, causando lentidão no carregamento da página</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Verificações de segurança que um registro é seu. Ex: Ao tentar acessar diretamente via URL um evento que não sou dono, o sistema abre a tela de edição sem verificar a propriedade do registro. O mesmo erro ocorre para os outros cadastros</t>
+  </si>
+  <si>
+    <t>Correção do bug na exibição de imagens da rota caso não existissem</t>
   </si>
 </sst>
 </file>
@@ -296,7 +313,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -336,6 +353,18 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -373,23 +402,33 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -448,11 +487,119 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="12">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -910,30 +1057,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="41.25" customHeight="1">
       <c r="B1" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -950,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="39">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -967,37 +1114,41 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="26">
       <c r="A7" s="9">
         <v>2</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="C7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="26">
       <c r="A8" s="6">
         <v>3</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="C8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>41</v>
+      <c r="D8" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="26">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1012,7 +1163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="26">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1029,7 +1180,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="52">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1051,39 +1202,45 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:B11">
-    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView showGridLines="0" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="41.25" customHeight="1">
       <c r="B1" s="21" t="s">
         <v>53</v>
       </c>
@@ -1091,7 +1248,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1111,7 +1268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="78">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1129,7 +1286,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="65">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1145,7 +1302,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="38.25" customHeight="1">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1161,7 +1318,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="39">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1177,7 +1334,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="39">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1193,7 +1350,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="26">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1213,7 +1370,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="65">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -1231,7 +1388,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="102" customHeight="1">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -1247,7 +1404,7 @@
       </c>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="52">
       <c r="A14" s="6">
         <v>9</v>
       </c>
@@ -1263,7 +1420,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="89.25" customHeight="1">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -1279,7 +1436,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="76.5" customHeight="1">
       <c r="A16" s="6">
         <v>11</v>
       </c>
@@ -1295,7 +1452,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="102" customHeight="1">
       <c r="A17" s="9">
         <v>12</v>
       </c>
@@ -1311,7 +1468,7 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="65">
       <c r="A18" s="6">
         <v>13</v>
       </c>
@@ -1327,7 +1484,7 @@
       </c>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="114.75" customHeight="1">
       <c r="A19" s="9">
         <v>14</v>
       </c>
@@ -1343,7 +1500,7 @@
       </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="63.75" customHeight="1">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -1359,7 +1516,7 @@
       </c>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="26">
       <c r="A21" s="9">
         <v>16</v>
       </c>
@@ -1377,7 +1534,7 @@
       </c>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="6">
         <v>17</v>
       </c>
@@ -1393,7 +1550,7 @@
       </c>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="9">
         <v>18</v>
       </c>
@@ -1409,7 +1566,7 @@
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="6">
         <v>19</v>
       </c>
@@ -1425,7 +1582,7 @@
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="26">
       <c r="A25" s="9">
         <v>20</v>
       </c>
@@ -1443,7 +1600,7 @@
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="26">
       <c r="A26" s="6">
         <v>21</v>
       </c>
@@ -1461,7 +1618,7 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="39">
       <c r="A27" s="9">
         <v>22</v>
       </c>
@@ -1477,7 +1634,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="26">
       <c r="A28" s="6">
         <v>23</v>
       </c>
@@ -1495,7 +1652,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="26">
       <c r="A29" s="9">
         <v>24</v>
       </c>
@@ -1513,7 +1670,7 @@
       </c>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="6">
         <v>25</v>
       </c>
@@ -1531,7 +1688,7 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="65">
       <c r="A31" s="9">
         <v>26</v>
       </c>
@@ -1547,7 +1704,7 @@
       </c>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="39">
       <c r="A32" s="6">
         <v>27</v>
       </c>
@@ -1563,7 +1720,7 @@
       </c>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="26">
       <c r="A33" s="9">
         <v>28</v>
       </c>
@@ -1579,7 +1736,7 @@
       </c>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="63.75" customHeight="1">
       <c r="A34" s="6">
         <v>29</v>
       </c>
@@ -1597,7 +1754,7 @@
       </c>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="26">
       <c r="A35" s="9">
         <v>30</v>
       </c>
@@ -1615,7 +1772,7 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="26">
       <c r="A36" s="6">
         <v>31</v>
       </c>
@@ -1633,7 +1790,7 @@
       </c>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="26">
       <c r="A37" s="9">
         <v>32</v>
       </c>
@@ -1649,7 +1806,7 @@
       </c>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" s="6">
         <v>33</v>
       </c>
@@ -1667,7 +1824,7 @@
       </c>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="39">
       <c r="A39" s="9">
         <v>34</v>
       </c>
@@ -1683,7 +1840,7 @@
       </c>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="26">
       <c r="A40" s="6">
         <v>35</v>
       </c>
@@ -1699,7 +1856,7 @@
       </c>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="26">
       <c r="A41" s="9">
         <v>36</v>
       </c>
@@ -1715,7 +1872,7 @@
       </c>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" s="9">
         <v>36</v>
       </c>
@@ -1731,7 +1888,7 @@
       </c>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" s="9">
         <v>37</v>
       </c>
@@ -1747,7 +1904,7 @@
       </c>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" s="9">
         <v>38</v>
       </c>
@@ -1763,7 +1920,7 @@
       </c>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="26">
       <c r="A45" s="9">
         <v>39</v>
       </c>
@@ -1778,6 +1935,58 @@
         <v>70</v>
       </c>
       <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" ht="52">
+      <c r="A46" s="9">
+        <v>40</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" ht="26">
+      <c r="A47" s="9">
+        <v>41</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="9">
+        <v>42</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:F45"/>
@@ -1786,47 +1995,76 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B6:B41">
-    <cfRule type="cellIs" dxfId="9" priority="29" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="23" priority="35" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="36" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="7" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="23" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="5" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="3" priority="13" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="1" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustes para o apontamento de listar Usuários que participam de um evento na Web.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\fusioness\Trunk\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="140" windowWidth="20940" windowHeight="16720"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="20940" windowHeight="16725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5" sheetId="2" r:id="rId1"/>
     <sheet name="To-do list" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$F$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$F$48</definedName>
   </definedNames>
   <calcPr calcId="101716" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="79">
   <si>
     <t>Responsável</t>
   </si>
@@ -304,6 +309,9 @@
   </si>
   <si>
     <t>Correção do bug na exibição de imagens da rota caso não existissem</t>
+  </si>
+  <si>
+    <t>Falta ainda adicionar os detalhes de cada usuário num Popup.</t>
   </si>
 </sst>
 </file>
@@ -313,7 +321,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -364,6 +372,12 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -430,7 +444,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -486,78 +500,25 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -1057,30 +1018,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41.25" customHeight="1">
+    <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1097,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="39">
+    <row r="6" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1114,7 +1075,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26">
+    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1131,7 +1092,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="26">
+    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1148,7 +1109,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="26">
+    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1163,7 +1124,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="26">
+    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1180,7 +1141,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="52">
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1202,10 +1163,10 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:B11">
-    <cfRule type="cellIs" dxfId="25" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1221,26 +1182,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="46.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="41.25" customHeight="1">
+    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="21" t="s">
         <v>53</v>
       </c>
@@ -1248,7 +1210,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1268,7 +1230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="78">
+    <row r="6" spans="1:6" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1286,7 +1248,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="65">
+    <row r="7" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1302,7 +1264,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="38.25" customHeight="1">
+    <row r="8" spans="1:6" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1318,7 +1280,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="39">
+    <row r="9" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1334,7 +1296,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="39">
+    <row r="10" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1350,7 +1312,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="26">
+    <row r="11" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1370,7 +1332,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="65">
+    <row r="12" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -1388,7 +1350,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="102" customHeight="1">
+    <row r="13" spans="1:6" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -1404,7 +1366,7 @@
       </c>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="52">
+    <row r="14" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>9</v>
       </c>
@@ -1420,7 +1382,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="89.25" customHeight="1">
+    <row r="15" spans="1:6" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -1436,7 +1398,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="76.5" customHeight="1">
+    <row r="16" spans="1:6" ht="76.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>11</v>
       </c>
@@ -1452,7 +1414,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="102" customHeight="1">
+    <row r="17" spans="1:6" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>12</v>
       </c>
@@ -1468,7 +1430,7 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" ht="65">
+    <row r="18" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>13</v>
       </c>
@@ -1484,7 +1446,7 @@
       </c>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="114.75" customHeight="1">
+    <row r="19" spans="1:6" ht="114.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>14</v>
       </c>
@@ -1500,7 +1462,7 @@
       </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="63.75" customHeight="1">
+    <row r="20" spans="1:6" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -1516,7 +1478,7 @@
       </c>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="26">
+    <row r="21" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>16</v>
       </c>
@@ -1534,7 +1496,7 @@
       </c>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>17</v>
       </c>
@@ -1550,7 +1512,7 @@
       </c>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>18</v>
       </c>
@@ -1566,7 +1528,7 @@
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>19</v>
       </c>
@@ -1582,7 +1544,7 @@
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" ht="26">
+    <row r="25" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>20</v>
       </c>
@@ -1600,7 +1562,7 @@
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" ht="26">
+    <row r="26" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>21</v>
       </c>
@@ -1618,7 +1580,7 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" ht="39">
+    <row r="27" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>22</v>
       </c>
@@ -1634,7 +1596,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" ht="26">
+    <row r="28" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>23</v>
       </c>
@@ -1652,7 +1614,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" ht="26">
+    <row r="29" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>24</v>
       </c>
@@ -1670,7 +1632,7 @@
       </c>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>25</v>
       </c>
@@ -1688,7 +1650,7 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" ht="65">
+    <row r="31" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>26</v>
       </c>
@@ -1704,7 +1666,7 @@
       </c>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" ht="39">
+    <row r="32" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>27</v>
       </c>
@@ -1720,7 +1682,7 @@
       </c>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" ht="26">
+    <row r="33" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>28</v>
       </c>
@@ -1736,7 +1698,7 @@
       </c>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" ht="63.75" customHeight="1">
+    <row r="34" spans="1:6" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>29</v>
       </c>
@@ -1754,7 +1716,7 @@
       </c>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="26">
+    <row r="35" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>30</v>
       </c>
@@ -1772,7 +1734,7 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" ht="26">
+    <row r="36" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>31</v>
       </c>
@@ -1790,7 +1752,7 @@
       </c>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="26">
+    <row r="37" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>32</v>
       </c>
@@ -1806,7 +1768,7 @@
       </c>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>33</v>
       </c>
@@ -1824,7 +1786,7 @@
       </c>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" ht="39">
+    <row r="39" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
         <v>34</v>
       </c>
@@ -1840,11 +1802,13 @@
       </c>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="26">
+    <row r="40" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>35</v>
       </c>
-      <c r="B40" s="9"/>
+      <c r="B40" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C40" s="12" t="s">
         <v>69</v>
       </c>
@@ -1852,11 +1816,13 @@
         <v>66</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="1:6" ht="26">
+        <v>41</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>36</v>
       </c>
@@ -1872,7 +1838,7 @@
       </c>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
         <v>36</v>
       </c>
@@ -1888,12 +1854,12 @@
       </c>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>37</v>
       </c>
       <c r="B43" s="9"/>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="23" t="s">
         <v>71</v>
       </c>
       <c r="D43" s="20" t="s">
@@ -1904,11 +1870,13 @@
       </c>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
         <v>38</v>
       </c>
-      <c r="B44" s="9"/>
+      <c r="B44" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C44" s="11" t="s">
         <v>72</v>
       </c>
@@ -1920,7 +1888,7 @@
       </c>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" ht="26">
+    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
         <v>39</v>
       </c>
@@ -1936,7 +1904,7 @@
       </c>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" ht="52">
+    <row r="46" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
         <v>40</v>
       </c>
@@ -1952,7 +1920,7 @@
       </c>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" ht="26">
+    <row r="47" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
         <v>41</v>
       </c>
@@ -1970,7 +1938,7 @@
       </c>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>42</v>
       </c>
@@ -1989,77 +1957,81 @@
       <c r="F48" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:F45"/>
+  <autoFilter ref="A5:F48">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B6:B41">
-    <cfRule type="cellIs" dxfId="23" priority="35" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="35" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="36" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="21" priority="23" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="23" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="24" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="19" priority="21" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="22" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="17" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="20" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="15" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Ajustes de bugs e funcionalidades. Descrito por email.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="20940" windowHeight="16725" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="20940" windowHeight="16725"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$F$48</definedName>
   </definedNames>
-  <calcPr calcId="101716" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="81">
   <si>
     <t>Responsável</t>
   </si>
@@ -248,15 +248,9 @@
     <t>Ao clicar num ponto de referência, poderá excluí-lo como um todo.</t>
   </si>
   <si>
-    <t>Deverá pegar todas as rotas que foram feitas a partir de uma rota original, e calcular a média de tempo entre elas.</t>
-  </si>
-  <si>
     <t>Verificar se é possível colocar mais informações relevantes.</t>
   </si>
   <si>
-    <t>Como combinado, o usuário fará uma espécie de Start do seu evento (via mobile), e pela WEB será possível acompanhar quanto tempo está levando cada usuário naquele evento em tempo real.</t>
-  </si>
-  <si>
     <t>Paulo</t>
   </si>
   <si>
@@ -296,9 +290,6 @@
     <t>Verificar o erro que aconteceu ao alterar um evento.</t>
   </si>
   <si>
-    <t>No lugar de escolher a rota para o evento, colocar uma seleção onde se possa ver os mapas das rotas possíveis.</t>
-  </si>
-  <si>
     <t>Remoção do hotlink das imagens de background, causando lentidão no carregamento da página</t>
   </si>
   <si>
@@ -312,6 +303,22 @@
   </si>
   <si>
     <t>Falta ainda adicionar os detalhes de cada usuário num Popup.</t>
+  </si>
+  <si>
+    <t>Como combinado, o usuário fará uma espécie de Start do seu evento (via mobile), e pela WEB será possível acompanhar quanto tempo está levando cada usuário naquele evento em tempo real. 
+Falta fazer um tratamento para exibir o tempo atual e o status de cada usuário no evento.</t>
+  </si>
+  <si>
+    <t>Ajustar bicicleta para que o cadastro da foto fique no proprio formulario de Inserir / Alterar. Usar como base a forma que foi feita para EVENTO.</t>
+  </si>
+  <si>
+    <t>Nas exclusões de Pontos de Referência e Imagem do Ponto, fazer aparecer a mensagem de confirmação que o registro foi excluído.</t>
+  </si>
+  <si>
+    <t>No lugar de escolher a rota para o evento, no momento que mudar a seleção da Rota, atualizar um mapa que deve ser colocado ao lado com as coordenadas daquela rota.</t>
+  </si>
+  <si>
+    <t>Após o ajuste que será feito em Rota, verificar onde vai ser exibida esta informação.</t>
   </si>
 </sst>
 </file>
@@ -321,7 +328,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -372,12 +379,6 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -444,7 +445,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -500,25 +501,50 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -730,9 +756,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -770,9 +796,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -807,7 +833,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -842,7 +868,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1018,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1080,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>35</v>
@@ -1097,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>37</v>
@@ -1109,7 +1135,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1118,10 +1144,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -1138,10 +1164,10 @@
         <v>43</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1155,7 +1181,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1163,10 +1189,10 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:B11">
-    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1183,10 +1209,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1221,7 +1247,7 @@
         <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>0</v>
@@ -1241,7 +1267,7 @@
         <v>45</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>40</v>
@@ -1292,7 +1318,7 @@
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" s="9"/>
     </row>
@@ -1323,13 +1349,13 @@
         <v>47</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>44</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
@@ -1343,7 +1369,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>40</v>
@@ -1378,7 +1404,7 @@
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F14" s="8"/>
     </row>
@@ -1489,26 +1515,28 @@
         <v>17</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>17</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C22" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F22" s="9"/>
     </row>
@@ -1555,10 +1583,10 @@
         <v>49</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F25" s="9"/>
     </row>
@@ -1573,10 +1601,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -1596,23 +1624,23 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>23</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="B28" s="9"/>
       <c r="C28" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
@@ -1625,7 +1653,7 @@
         <v>25</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>41</v>
@@ -1643,7 +1671,7 @@
         <v>24</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>41</v>
@@ -1659,10 +1687,10 @@
         <v>50</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F31" s="9"/>
     </row>
@@ -1709,7 +1737,7 @@
         <v>28</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>40</v>
@@ -1727,7 +1755,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>41</v>
@@ -1745,23 +1773,25 @@
         <v>30</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>32</v>
       </c>
-      <c r="B37" s="9"/>
+      <c r="B37" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C37" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>42</v>
@@ -1779,7 +1809,7 @@
         <v>31</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>42</v>
@@ -1795,14 +1825,14 @@
         <v>32</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>44</v>
       </c>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>35</v>
       </c>
@@ -1810,16 +1840,16 @@
         <v>1</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
@@ -1844,33 +1874,35 @@
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>70</v>
-      </c>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>37</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="23" t="s">
-        <v>71</v>
+      <c r="B43" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
         <v>38</v>
       </c>
@@ -1878,29 +1910,29 @@
         <v>1</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
         <v>39</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="11" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="F45" s="8"/>
     </row>
@@ -1910,13 +1942,13 @@
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F46" s="8"/>
     </row>
@@ -1925,13 +1957,13 @@
         <v>41</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>40</v>
@@ -1943,18 +1975,34 @@
         <v>42</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>40</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:F48">
@@ -1967,66 +2015,74 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B6:B41">
-    <cfRule type="cellIs" dxfId="15" priority="35" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="37" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="38" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="13" priority="23" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="25" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="26" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="11" priority="21" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="23" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="24" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="9" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="22" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="7" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removido o conceito de TipoRota que não faz mais parte do projeto. Adicionado tratamentos na página de Rota. Adicionada funcionalidade de Listar Rotas por Rota original usando ajax. Mais um monte de melhorias que não lembro de cabeça.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="20940" windowHeight="16725"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="20130" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
   <si>
     <t>Responsável</t>
   </si>
@@ -503,34 +503,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -756,9 +742,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -796,7 +782,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -868,7 +854,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1045,7 +1031,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1144,7 +1130,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>80</v>
@@ -1189,15 +1175,15 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:B11">
-    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1212,7 +1198,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1628,7 +1614,9 @@
       <c r="A28" s="6">
         <v>23</v>
       </c>
-      <c r="B28" s="9"/>
+      <c r="B28" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C28" s="11" t="s">
         <v>23</v>
       </c>
@@ -1682,7 +1670,9 @@
       <c r="A31" s="9">
         <v>26</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="C31" s="12" t="s">
         <v>50</v>
       </c>
@@ -2015,74 +2005,74 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B6:B41">
-    <cfRule type="cellIs" dxfId="19" priority="37" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="37" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="38" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="38" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="17" priority="25" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="25" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="26" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="15" priority="23" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="23" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="24" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" dxfId="13" priority="21" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="22" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="11" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="20" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finalização de US, correção de bugs, e melhorias
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
+++ b/Trunk/Doc/Planilha Atividades Sprint #5.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\fusioness\Trunk\Doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="20130" windowHeight="7620"/>
+    <workbookView xWindow="360" yWindow="140" windowWidth="20140" windowHeight="14180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 5" sheetId="2" r:id="rId1"/>
@@ -18,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To-do list'!$A$5:$F$48</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="81">
   <si>
     <t>Responsável</t>
   </si>
@@ -503,16 +498,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -784,7 +779,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -819,7 +814,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1030,30 +1025,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="41.25" customHeight="1">
       <c r="B1" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1070,7 +1065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="39">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1087,7 +1082,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="26">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1104,7 +1099,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="26">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1121,7 +1116,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="26">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1136,7 +1131,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="26">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1153,7 +1148,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="91">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1183,7 +1178,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1194,27 +1189,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="41.25" customHeight="1">
       <c r="B1" s="21" t="s">
         <v>53</v>
       </c>
@@ -1222,7 +1217,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1242,7 +1237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="78" hidden="1">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1260,7 +1255,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="65" hidden="1">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1276,7 +1271,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="38.25" hidden="1" customHeight="1">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -1292,7 +1287,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="39" hidden="1">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1308,7 +1303,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="39" hidden="1">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -1324,7 +1319,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="26" hidden="1">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1344,7 +1339,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="65" hidden="1">
       <c r="A12" s="6">
         <v>7</v>
       </c>
@@ -1362,7 +1357,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="102" hidden="1" customHeight="1">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -1378,7 +1373,7 @@
       </c>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="52" hidden="1">
       <c r="A14" s="6">
         <v>9</v>
       </c>
@@ -1394,7 +1389,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="89.25" hidden="1" customHeight="1">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -1410,7 +1405,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="76.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="76.5" hidden="1" customHeight="1">
       <c r="A16" s="6">
         <v>11</v>
       </c>
@@ -1426,7 +1421,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="102" hidden="1" customHeight="1">
       <c r="A17" s="9">
         <v>12</v>
       </c>
@@ -1442,7 +1437,7 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" ht="63.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="65" hidden="1">
       <c r="A18" s="6">
         <v>13</v>
       </c>
@@ -1458,7 +1453,7 @@
       </c>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="114.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="114.75" hidden="1" customHeight="1">
       <c r="A19" s="9">
         <v>14</v>
       </c>
@@ -1474,7 +1469,7 @@
       </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="63.75" hidden="1" customHeight="1">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -1490,7 +1485,7 @@
       </c>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="26" hidden="1">
       <c r="A21" s="9">
         <v>16</v>
       </c>
@@ -1508,7 +1503,7 @@
       </c>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" hidden="1">
       <c r="A22" s="6">
         <v>17</v>
       </c>
@@ -1526,7 +1521,7 @@
       </c>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" hidden="1">
       <c r="A23" s="9">
         <v>18</v>
       </c>
@@ -1542,7 +1537,7 @@
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" hidden="1">
       <c r="A24" s="6">
         <v>19</v>
       </c>
@@ -1558,7 +1553,7 @@
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="26" hidden="1">
       <c r="A25" s="9">
         <v>20</v>
       </c>
@@ -1576,7 +1571,7 @@
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="26" hidden="1">
       <c r="A26" s="6">
         <v>21</v>
       </c>
@@ -1594,7 +1589,7 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="39" hidden="1">
       <c r="A27" s="9">
         <v>22</v>
       </c>
@@ -1610,7 +1605,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="39">
       <c r="A28" s="6">
         <v>23</v>
       </c>
@@ -1630,7 +1625,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="26" hidden="1">
       <c r="A29" s="9">
         <v>24</v>
       </c>
@@ -1648,7 +1643,7 @@
       </c>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" hidden="1">
       <c r="A30" s="6">
         <v>25</v>
       </c>
@@ -1666,7 +1661,7 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="65">
       <c r="A31" s="9">
         <v>26</v>
       </c>
@@ -1684,7 +1679,7 @@
       </c>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="39" hidden="1">
       <c r="A32" s="6">
         <v>27</v>
       </c>
@@ -1700,7 +1695,7 @@
       </c>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="26" hidden="1">
       <c r="A33" s="9">
         <v>28</v>
       </c>
@@ -1716,7 +1711,7 @@
       </c>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="63.75" hidden="1" customHeight="1">
       <c r="A34" s="6">
         <v>29</v>
       </c>
@@ -1734,7 +1729,7 @@
       </c>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="26" hidden="1">
       <c r="A35" s="9">
         <v>30</v>
       </c>
@@ -1752,7 +1747,7 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="26" hidden="1">
       <c r="A36" s="6">
         <v>31</v>
       </c>
@@ -1770,7 +1765,7 @@
       </c>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="26" hidden="1">
       <c r="A37" s="9">
         <v>32</v>
       </c>
@@ -1788,7 +1783,7 @@
       </c>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" hidden="1">
       <c r="A38" s="6">
         <v>33</v>
       </c>
@@ -1806,7 +1801,7 @@
       </c>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="39">
       <c r="A39" s="9">
         <v>34</v>
       </c>
@@ -1822,7 +1817,7 @@
       </c>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="26" hidden="1">
       <c r="A40" s="6">
         <v>35</v>
       </c>
@@ -1842,7 +1837,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="26" hidden="1">
       <c r="A41" s="9">
         <v>36</v>
       </c>
@@ -1858,7 +1853,7 @@
       </c>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" s="9">
         <v>36</v>
       </c>
@@ -1874,7 +1869,7 @@
       </c>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" hidden="1">
       <c r="A43" s="9">
         <v>37</v>
       </c>
@@ -1892,7 +1887,7 @@
       </c>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" hidden="1">
       <c r="A44" s="9">
         <v>38</v>
       </c>
@@ -1910,11 +1905,13 @@
       </c>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="39">
       <c r="A45" s="9">
         <v>39</v>
       </c>
-      <c r="B45" s="9"/>
+      <c r="B45" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="C45" s="11" t="s">
         <v>79</v>
       </c>
@@ -1926,7 +1923,7 @@
       </c>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="52">
       <c r="A46" s="9">
         <v>40</v>
       </c>
@@ -1942,7 +1939,7 @@
       </c>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="26" hidden="1">
       <c r="A47" s="9">
         <v>41</v>
       </c>
@@ -1960,7 +1957,7 @@
       </c>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" hidden="1">
       <c r="A48" s="9">
         <v>42</v>
       </c>
@@ -1978,7 +1975,7 @@
       </c>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="26">
       <c r="A49" s="9">
         <v>40</v>
       </c>
@@ -2077,7 +2074,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>